<commit_message>
Removing old datasets for more tidy folders
</commit_message>
<xml_diff>
--- a/Data/Unemployment rate 2013-2023.xlsx
+++ b/Data/Unemployment rate 2013-2023.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ha_b_\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ha_b_\OneDrive\Documents\Skole\Assignments_MSB104\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB58B463-E4A0-427A-94A9-E078D0AC74CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925B017A-B94F-4204-8BD2-350C4567F490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="179">
   <si>
     <t>Unemployment rate by NUTS 2 region [tgs00010__custom_18888209]</t>
   </si>
@@ -2513,13 +2513,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M71"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="12" topLeftCell="C52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O19" sqref="O19"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2676,2310 +2676,2269 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="14">
-        <v>12.1</v>
-      </c>
-      <c r="D13" s="14">
-        <v>11.7</v>
-      </c>
-      <c r="E13" s="14">
-        <v>10.9</v>
-      </c>
-      <c r="F13" s="14">
-        <v>10.1</v>
-      </c>
-      <c r="G13" s="14">
-        <v>9.1</v>
-      </c>
-      <c r="H13" s="14">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="I13" s="14">
-        <v>7.5</v>
-      </c>
-      <c r="J13" s="14">
-        <v>7.9</v>
-      </c>
-      <c r="K13" s="14">
-        <v>7.8</v>
-      </c>
-      <c r="L13" s="14">
-        <v>6.8</v>
-      </c>
-      <c r="M13" s="14">
-        <v>6.6</v>
+        <v>40</v>
+      </c>
+      <c r="C13" s="15">
+        <v>3.7</v>
+      </c>
+      <c r="D13" s="15">
+        <v>3.1</v>
+      </c>
+      <c r="E13" s="15">
+        <v>3.4</v>
+      </c>
+      <c r="F13" s="15">
+        <v>3.3</v>
+      </c>
+      <c r="G13" s="19">
+        <v>3</v>
+      </c>
+      <c r="H13" s="15">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I13" s="15">
+        <v>2.4</v>
+      </c>
+      <c r="J13" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="K13" s="15">
+        <v>3.1</v>
+      </c>
+      <c r="L13" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="M13" s="15">
+        <v>2.9</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="15">
-        <v>3.7</v>
-      </c>
-      <c r="D14" s="15">
+        <v>42</v>
+      </c>
+      <c r="C14" s="14">
+        <v>3.6</v>
+      </c>
+      <c r="D14" s="14">
+        <v>3.5</v>
+      </c>
+      <c r="E14" s="14">
+        <v>3.3</v>
+      </c>
+      <c r="F14" s="14">
         <v>3.1</v>
       </c>
-      <c r="E14" s="15">
+      <c r="G14" s="14">
+        <v>3.3</v>
+      </c>
+      <c r="H14" s="18">
+        <v>3</v>
+      </c>
+      <c r="I14" s="14">
+        <v>2.8</v>
+      </c>
+      <c r="J14" s="14">
+        <v>3.5</v>
+      </c>
+      <c r="K14" s="14">
         <v>3.4</v>
       </c>
-      <c r="F14" s="15">
-        <v>3.3</v>
-      </c>
-      <c r="G14" s="19">
-        <v>3</v>
-      </c>
-      <c r="H14" s="15">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="I14" s="15">
-        <v>2.4</v>
-      </c>
-      <c r="J14" s="15">
-        <v>3.5</v>
-      </c>
-      <c r="K14" s="15">
-        <v>3.1</v>
-      </c>
-      <c r="L14" s="15">
-        <v>2.8</v>
-      </c>
-      <c r="M14" s="15">
+      <c r="L14" s="14">
+        <v>3.2</v>
+      </c>
+      <c r="M14" s="14">
         <v>2.9</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="14">
-        <v>3.6</v>
-      </c>
-      <c r="D15" s="14">
-        <v>3.5</v>
-      </c>
-      <c r="E15" s="14">
-        <v>3.3</v>
-      </c>
-      <c r="F15" s="14">
-        <v>3.1</v>
-      </c>
-      <c r="G15" s="14">
-        <v>3.3</v>
-      </c>
-      <c r="H15" s="18">
+        <v>44</v>
+      </c>
+      <c r="C15" s="15">
+        <v>2.9</v>
+      </c>
+      <c r="D15" s="19">
         <v>3</v>
       </c>
-      <c r="I15" s="14">
-        <v>2.8</v>
-      </c>
-      <c r="J15" s="14">
-        <v>3.5</v>
-      </c>
-      <c r="K15" s="14">
-        <v>3.4</v>
-      </c>
-      <c r="L15" s="14">
+      <c r="E15" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="F15" s="19">
+        <v>3</v>
+      </c>
+      <c r="G15" s="15">
+        <v>2.9</v>
+      </c>
+      <c r="H15" s="15">
+        <v>2.6</v>
+      </c>
+      <c r="I15" s="15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J15" s="15">
+        <v>2.7</v>
+      </c>
+      <c r="K15" s="15">
         <v>3.2</v>
       </c>
-      <c r="M15" s="14">
-        <v>2.9</v>
+      <c r="L15" s="15">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="M15" s="15">
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="15">
+        <v>46</v>
+      </c>
+      <c r="C16" s="14">
         <v>2.9</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="14">
+        <v>2.7</v>
+      </c>
+      <c r="E16" s="18">
         <v>3</v>
       </c>
-      <c r="E16" s="15">
-        <v>2.5</v>
-      </c>
-      <c r="F16" s="19">
+      <c r="F16" s="14">
+        <v>2.6</v>
+      </c>
+      <c r="G16" s="14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H16" s="14">
+        <v>1.9</v>
+      </c>
+      <c r="I16" s="14">
+        <v>1.9</v>
+      </c>
+      <c r="J16" s="14">
+        <v>2.9</v>
+      </c>
+      <c r="K16" s="18">
         <v>3</v>
       </c>
-      <c r="G16" s="15">
-        <v>2.9</v>
-      </c>
-      <c r="H16" s="15">
-        <v>2.6</v>
-      </c>
-      <c r="I16" s="15">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="J16" s="15">
-        <v>2.7</v>
-      </c>
-      <c r="K16" s="15">
-        <v>3.2</v>
-      </c>
-      <c r="L16" s="15">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="M16" s="15">
-        <v>2.2000000000000002</v>
+      <c r="L16" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="M16" s="14">
+        <v>2.1</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="14">
-        <v>2.9</v>
-      </c>
-      <c r="D17" s="14">
+        <v>48</v>
+      </c>
+      <c r="C17" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="D17" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="E17" s="15">
         <v>2.7</v>
       </c>
-      <c r="E17" s="18">
-        <v>3</v>
-      </c>
-      <c r="F17" s="14">
-        <v>2.6</v>
-      </c>
-      <c r="G17" s="14">
+      <c r="F17" s="15">
+        <v>2.4</v>
+      </c>
+      <c r="G17" s="15">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="15">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I17" s="15">
         <v>1.9</v>
       </c>
-      <c r="I17" s="14">
-        <v>1.9</v>
-      </c>
-      <c r="J17" s="14">
-        <v>2.9</v>
-      </c>
-      <c r="K17" s="18">
-        <v>3</v>
-      </c>
-      <c r="L17" s="14">
-        <v>2.1</v>
-      </c>
-      <c r="M17" s="14">
-        <v>2.1</v>
+      <c r="J17" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="K17" s="15">
+        <v>2.7</v>
+      </c>
+      <c r="L17" s="15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M17" s="15">
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="15">
+        <v>50</v>
+      </c>
+      <c r="C18" s="14">
+        <v>3.2</v>
+      </c>
+      <c r="D18" s="14">
+        <v>2.9</v>
+      </c>
+      <c r="E18" s="14">
         <v>2.5</v>
       </c>
-      <c r="D18" s="15">
-        <v>2.5</v>
-      </c>
-      <c r="E18" s="15">
-        <v>2.7</v>
-      </c>
-      <c r="F18" s="15">
-        <v>2.4</v>
-      </c>
-      <c r="G18" s="15">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H18" s="15">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="I18" s="15">
-        <v>1.9</v>
-      </c>
-      <c r="J18" s="15">
-        <v>2.8</v>
-      </c>
-      <c r="K18" s="15">
-        <v>2.7</v>
-      </c>
-      <c r="L18" s="15">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M18" s="15">
-        <v>2.2999999999999998</v>
+      <c r="F18" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="G18" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="H18" s="18">
+        <v>2</v>
+      </c>
+      <c r="I18" s="18">
+        <v>2</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="K18" s="14">
+        <v>1.8</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="14">
-        <v>3.2</v>
-      </c>
-      <c r="D19" s="14">
+        <v>52</v>
+      </c>
+      <c r="C19" s="15">
+        <v>3.4</v>
+      </c>
+      <c r="D19" s="15">
+        <v>2.7</v>
+      </c>
+      <c r="E19" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="F19" s="15">
         <v>2.9</v>
       </c>
-      <c r="E19" s="14">
-        <v>2.5</v>
-      </c>
-      <c r="F19" s="14">
+      <c r="G19" s="15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H19" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="I19" s="15">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="K19" s="15">
+        <v>2.4</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="M19" s="15">
         <v>2.1</v>
-      </c>
-      <c r="G19" s="14">
-        <v>2.1</v>
-      </c>
-      <c r="H19" s="18">
-        <v>2</v>
-      </c>
-      <c r="I19" s="18">
-        <v>2</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="K19" s="14">
-        <v>1.8</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="M19" s="7" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="15">
-        <v>3.4</v>
-      </c>
-      <c r="D20" s="15">
-        <v>2.7</v>
-      </c>
-      <c r="E20" s="15">
-        <v>2.8</v>
-      </c>
-      <c r="F20" s="15">
-        <v>2.9</v>
-      </c>
-      <c r="G20" s="15">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H20" s="15">
-        <v>1.9</v>
-      </c>
-      <c r="I20" s="15">
+        <v>54</v>
+      </c>
+      <c r="C20" s="14">
+        <v>3.9</v>
+      </c>
+      <c r="D20" s="18">
+        <v>4</v>
+      </c>
+      <c r="E20" s="14">
+        <v>3.9</v>
+      </c>
+      <c r="F20" s="14">
+        <v>3.3</v>
+      </c>
+      <c r="G20" s="18">
+        <v>3</v>
+      </c>
+      <c r="H20" s="14">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="I20" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J20" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="K20" s="15">
-        <v>2.4</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="M20" s="15">
-        <v>2.1</v>
+      <c r="K20" s="14">
+        <v>3.3</v>
+      </c>
+      <c r="L20" s="18">
+        <v>3</v>
+      </c>
+      <c r="M20" s="14">
+        <v>2.5</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="14">
-        <v>3.9</v>
-      </c>
-      <c r="D21" s="18">
-        <v>4</v>
-      </c>
-      <c r="E21" s="14">
-        <v>3.9</v>
-      </c>
-      <c r="F21" s="14">
-        <v>3.3</v>
-      </c>
-      <c r="G21" s="18">
+        <v>56</v>
+      </c>
+      <c r="C21" s="15">
+        <v>3.1</v>
+      </c>
+      <c r="D21" s="15">
+        <v>3.1</v>
+      </c>
+      <c r="E21" s="19">
         <v>3</v>
       </c>
-      <c r="H21" s="14">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="I21" s="14">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="K21" s="14">
-        <v>3.3</v>
-      </c>
-      <c r="L21" s="18">
-        <v>3</v>
-      </c>
-      <c r="M21" s="14">
+      <c r="F21" s="15">
         <v>2.5</v>
+      </c>
+      <c r="G21" s="15">
+        <v>2.1</v>
+      </c>
+      <c r="H21" s="15">
+        <v>1.8</v>
+      </c>
+      <c r="I21" s="15">
+        <v>2.1</v>
+      </c>
+      <c r="J21" s="15">
+        <v>3.8</v>
+      </c>
+      <c r="K21" s="15">
+        <v>3.4</v>
+      </c>
+      <c r="L21" s="15">
+        <v>2.9</v>
+      </c>
+      <c r="M21" s="15">
+        <v>2.4</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="15">
-        <v>3.1</v>
-      </c>
-      <c r="D22" s="15">
-        <v>3.1</v>
-      </c>
-      <c r="E22" s="19">
+        <v>58</v>
+      </c>
+      <c r="C22" s="14">
+        <v>3.3</v>
+      </c>
+      <c r="D22" s="14">
+        <v>2.9</v>
+      </c>
+      <c r="E22" s="18">
         <v>3</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="14">
         <v>2.5</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H22" s="18">
+        <v>2</v>
+      </c>
+      <c r="I22" s="18">
+        <v>2</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="K22" s="14">
+        <v>2.6</v>
+      </c>
+      <c r="L22" s="14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M22" s="14">
         <v>2.1</v>
-      </c>
-      <c r="H22" s="15">
-        <v>1.8</v>
-      </c>
-      <c r="I22" s="15">
-        <v>2.1</v>
-      </c>
-      <c r="J22" s="15">
-        <v>3.8</v>
-      </c>
-      <c r="K22" s="15">
-        <v>3.4</v>
-      </c>
-      <c r="L22" s="15">
-        <v>2.9</v>
-      </c>
-      <c r="M22" s="15">
-        <v>2.4</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="14">
+        <v>60</v>
+      </c>
+      <c r="C23" s="15">
         <v>3.3</v>
       </c>
-      <c r="D23" s="14">
-        <v>2.9</v>
-      </c>
-      <c r="E23" s="18">
+      <c r="D23" s="19">
         <v>3</v>
       </c>
-      <c r="F23" s="14">
+      <c r="E23" s="19">
+        <v>3</v>
+      </c>
+      <c r="F23" s="15">
+        <v>2.7</v>
+      </c>
+      <c r="G23" s="15">
+        <v>2.6</v>
+      </c>
+      <c r="H23" s="15">
+        <v>2.4</v>
+      </c>
+      <c r="I23" s="15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J23" s="15">
         <v>2.5</v>
       </c>
-      <c r="G23" s="14">
+      <c r="K23" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="L23" s="15">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H23" s="18">
-        <v>2</v>
-      </c>
-      <c r="I23" s="18">
-        <v>2</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="K23" s="14">
-        <v>2.6</v>
-      </c>
-      <c r="L23" s="14">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M23" s="14">
-        <v>2.1</v>
+      <c r="M23" s="15">
+        <v>1.8</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="15">
-        <v>3.3</v>
-      </c>
-      <c r="D24" s="19">
-        <v>3</v>
-      </c>
-      <c r="E24" s="19">
-        <v>3</v>
-      </c>
-      <c r="F24" s="15">
-        <v>2.7</v>
-      </c>
-      <c r="G24" s="15">
-        <v>2.6</v>
-      </c>
-      <c r="H24" s="15">
-        <v>2.4</v>
-      </c>
-      <c r="I24" s="15">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="J24" s="15">
-        <v>2.5</v>
-      </c>
-      <c r="K24" s="15">
-        <v>2.8</v>
-      </c>
-      <c r="L24" s="15">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="M24" s="15">
-        <v>1.8</v>
+        <v>62</v>
+      </c>
+      <c r="C24" s="14">
+        <v>10.4</v>
+      </c>
+      <c r="D24" s="14">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E24" s="14">
+        <v>9.5</v>
+      </c>
+      <c r="F24" s="14">
+        <v>7.8</v>
+      </c>
+      <c r="G24" s="18">
+        <v>7</v>
+      </c>
+      <c r="H24" s="14">
+        <v>6.1</v>
+      </c>
+      <c r="I24" s="14">
+        <v>5.3</v>
+      </c>
+      <c r="J24" s="14">
+        <v>6.1</v>
+      </c>
+      <c r="K24" s="14">
+        <v>5.7</v>
+      </c>
+      <c r="L24" s="14">
+        <v>4.8</v>
+      </c>
+      <c r="M24" s="14">
+        <v>5.2</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="14">
-        <v>10.4</v>
-      </c>
-      <c r="D25" s="14">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="E25" s="14">
-        <v>9.5</v>
-      </c>
-      <c r="F25" s="14">
-        <v>7.8</v>
-      </c>
-      <c r="G25" s="18">
-        <v>7</v>
-      </c>
-      <c r="H25" s="14">
-        <v>6.1</v>
-      </c>
-      <c r="I25" s="14">
-        <v>5.3</v>
-      </c>
-      <c r="J25" s="14">
-        <v>6.1</v>
-      </c>
-      <c r="K25" s="14">
+        <v>64</v>
+      </c>
+      <c r="C25" s="15">
+        <v>7.3</v>
+      </c>
+      <c r="D25" s="15">
+        <v>6.7</v>
+      </c>
+      <c r="E25" s="15">
         <v>5.7</v>
       </c>
-      <c r="L25" s="14">
-        <v>4.8</v>
-      </c>
-      <c r="M25" s="14">
-        <v>5.2</v>
+      <c r="F25" s="15">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G25" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="H25" s="15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I25" s="15">
+        <v>3.4</v>
+      </c>
+      <c r="J25" s="15">
+        <v>4.2</v>
+      </c>
+      <c r="K25" s="19">
+        <v>3</v>
+      </c>
+      <c r="L25" s="15">
+        <v>3.3</v>
+      </c>
+      <c r="M25" s="15">
+        <v>3.3</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="15">
-        <v>7.3</v>
-      </c>
-      <c r="D26" s="15">
-        <v>6.7</v>
-      </c>
-      <c r="E26" s="15">
-        <v>5.7</v>
-      </c>
-      <c r="F26" s="15">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="G26" s="15">
-        <v>4.5</v>
-      </c>
-      <c r="H26" s="15">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="I26" s="15">
-        <v>3.4</v>
-      </c>
-      <c r="J26" s="15">
-        <v>4.2</v>
-      </c>
-      <c r="K26" s="19">
-        <v>3</v>
-      </c>
-      <c r="L26" s="15">
-        <v>3.3</v>
-      </c>
-      <c r="M26" s="15">
-        <v>3.3</v>
+        <v>66</v>
+      </c>
+      <c r="C26" s="18">
+        <v>7</v>
+      </c>
+      <c r="D26" s="14">
+        <v>6.6</v>
+      </c>
+      <c r="E26" s="14">
+        <v>5.6</v>
+      </c>
+      <c r="F26" s="14">
+        <v>5.4</v>
+      </c>
+      <c r="G26" s="14">
+        <v>4.3</v>
+      </c>
+      <c r="H26" s="14">
+        <v>4.3</v>
+      </c>
+      <c r="I26" s="14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="K26" s="14">
+        <v>6.5</v>
+      </c>
+      <c r="L26" s="14">
+        <v>5.6</v>
+      </c>
+      <c r="M26" s="14">
+        <v>4.7</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="18">
-        <v>7</v>
-      </c>
-      <c r="D27" s="14">
-        <v>6.6</v>
-      </c>
-      <c r="E27" s="14">
-        <v>5.6</v>
-      </c>
-      <c r="F27" s="14">
-        <v>5.4</v>
-      </c>
-      <c r="G27" s="14">
+        <v>68</v>
+      </c>
+      <c r="C27" s="15">
+        <v>4.7</v>
+      </c>
+      <c r="D27" s="19">
+        <v>5</v>
+      </c>
+      <c r="E27" s="15">
         <v>4.3</v>
       </c>
-      <c r="H27" s="14">
-        <v>4.3</v>
-      </c>
-      <c r="I27" s="14">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="K27" s="14">
-        <v>6.5</v>
-      </c>
-      <c r="L27" s="14">
-        <v>5.6</v>
-      </c>
-      <c r="M27" s="14">
-        <v>4.7</v>
+      <c r="F27" s="15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G27" s="15">
+        <v>4.2</v>
+      </c>
+      <c r="H27" s="15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I27" s="15">
+        <v>3.6</v>
+      </c>
+      <c r="J27" s="15">
+        <v>4.8</v>
+      </c>
+      <c r="K27" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="L27" s="19">
+        <v>4</v>
+      </c>
+      <c r="M27" s="15">
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="15">
-        <v>4.7</v>
-      </c>
-      <c r="D28" s="19">
-        <v>5</v>
-      </c>
-      <c r="E28" s="15">
+        <v>70</v>
+      </c>
+      <c r="C28" s="14">
         <v>4.3</v>
       </c>
-      <c r="F28" s="15">
+      <c r="D28" s="14">
+        <v>4.5</v>
+      </c>
+      <c r="E28" s="14">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G28" s="15">
+      <c r="F28" s="18">
+        <v>4</v>
+      </c>
+      <c r="G28" s="14">
+        <v>3.5</v>
+      </c>
+      <c r="H28" s="14">
+        <v>3.1</v>
+      </c>
+      <c r="I28" s="14">
+        <v>3.1</v>
+      </c>
+      <c r="J28" s="14">
         <v>4.2</v>
       </c>
-      <c r="H28" s="15">
+      <c r="K28" s="14">
         <v>4.0999999999999996</v>
       </c>
-      <c r="I28" s="15">
-        <v>3.6</v>
-      </c>
-      <c r="J28" s="15">
-        <v>4.8</v>
-      </c>
-      <c r="K28" s="15">
-        <v>4.5</v>
-      </c>
-      <c r="L28" s="19">
-        <v>4</v>
-      </c>
-      <c r="M28" s="15">
-        <v>4.0999999999999996</v>
+      <c r="L28" s="14">
+        <v>3.9</v>
+      </c>
+      <c r="M28" s="14">
+        <v>3.1</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C29" s="14">
-        <v>4.3</v>
-      </c>
-      <c r="D29" s="14">
+        <v>72</v>
+      </c>
+      <c r="C29" s="15">
         <v>4.5</v>
       </c>
-      <c r="E29" s="14">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="F29" s="18">
+      <c r="D29" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="E29" s="15">
+        <v>3.9</v>
+      </c>
+      <c r="F29" s="19">
         <v>4</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="15">
+        <v>3.6</v>
+      </c>
+      <c r="H29" s="15">
+        <v>3.6</v>
+      </c>
+      <c r="I29" s="15">
+        <v>3.3</v>
+      </c>
+      <c r="J29" s="15">
+        <v>5.2</v>
+      </c>
+      <c r="K29" s="15">
         <v>3.5</v>
       </c>
-      <c r="H29" s="14">
-        <v>3.1</v>
-      </c>
-      <c r="I29" s="14">
-        <v>3.1</v>
-      </c>
-      <c r="J29" s="14">
-        <v>4.2</v>
-      </c>
-      <c r="K29" s="14">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="L29" s="14">
-        <v>3.9</v>
-      </c>
-      <c r="M29" s="14">
-        <v>3.1</v>
+      <c r="L29" s="15">
+        <v>2.6</v>
+      </c>
+      <c r="M29" s="19">
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="15">
-        <v>4.5</v>
-      </c>
-      <c r="D30" s="15">
-        <v>4.5</v>
-      </c>
-      <c r="E30" s="15">
-        <v>3.9</v>
-      </c>
-      <c r="F30" s="19">
-        <v>4</v>
-      </c>
-      <c r="G30" s="15">
+        <v>74</v>
+      </c>
+      <c r="C30" s="14">
+        <v>4.3</v>
+      </c>
+      <c r="D30" s="14">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E30" s="14">
         <v>3.6</v>
       </c>
-      <c r="H30" s="15">
-        <v>3.6</v>
-      </c>
-      <c r="I30" s="15">
-        <v>3.3</v>
-      </c>
-      <c r="J30" s="15">
-        <v>5.2</v>
-      </c>
-      <c r="K30" s="15">
-        <v>3.5</v>
-      </c>
-      <c r="L30" s="15">
-        <v>2.6</v>
-      </c>
-      <c r="M30" s="19">
+      <c r="F30" s="14">
+        <v>3.7</v>
+      </c>
+      <c r="G30" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="H30" s="14">
+        <v>2.9</v>
+      </c>
+      <c r="I30" s="14">
+        <v>2.8</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="K30" s="18">
         <v>3</v>
+      </c>
+      <c r="L30" s="14">
+        <v>2.4</v>
+      </c>
+      <c r="M30" s="14">
+        <v>2.1</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C31" s="14">
+        <v>76</v>
+      </c>
+      <c r="C31" s="15">
+        <v>10.1</v>
+      </c>
+      <c r="D31" s="15">
+        <v>9.6</v>
+      </c>
+      <c r="E31" s="15">
+        <v>7.8</v>
+      </c>
+      <c r="F31" s="15">
+        <v>6.3</v>
+      </c>
+      <c r="G31" s="15">
+        <v>5.2</v>
+      </c>
+      <c r="H31" s="15">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I31" s="19">
+        <v>4</v>
+      </c>
+      <c r="J31" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="K31" s="15">
+        <v>3.8</v>
+      </c>
+      <c r="L31" s="15">
+        <v>3.8</v>
+      </c>
+      <c r="M31" s="15">
         <v>4.3</v>
-      </c>
-      <c r="D31" s="14">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E31" s="14">
-        <v>3.6</v>
-      </c>
-      <c r="F31" s="14">
-        <v>3.7</v>
-      </c>
-      <c r="G31" s="14">
-        <v>2.5</v>
-      </c>
-      <c r="H31" s="14">
-        <v>2.9</v>
-      </c>
-      <c r="I31" s="14">
-        <v>2.8</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="K31" s="18">
-        <v>3</v>
-      </c>
-      <c r="L31" s="14">
-        <v>2.4</v>
-      </c>
-      <c r="M31" s="14">
-        <v>2.1</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="15">
-        <v>10.1</v>
-      </c>
-      <c r="D32" s="15">
-        <v>9.6</v>
-      </c>
-      <c r="E32" s="15">
-        <v>7.8</v>
-      </c>
-      <c r="F32" s="15">
-        <v>6.3</v>
-      </c>
-      <c r="G32" s="15">
-        <v>5.2</v>
-      </c>
-      <c r="H32" s="15">
+        <v>78</v>
+      </c>
+      <c r="C32" s="14">
+        <v>6.2</v>
+      </c>
+      <c r="D32" s="14">
+        <v>5.5</v>
+      </c>
+      <c r="E32" s="14">
         <v>4.9000000000000004</v>
       </c>
-      <c r="I32" s="19">
+      <c r="F32" s="14">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G32" s="14">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H32" s="18">
         <v>4</v>
       </c>
-      <c r="J32" s="15">
+      <c r="I32" s="14">
+        <v>3.3</v>
+      </c>
+      <c r="J32" s="14">
         <v>4.5</v>
       </c>
-      <c r="K32" s="15">
-        <v>3.8</v>
-      </c>
-      <c r="L32" s="15">
-        <v>3.8</v>
-      </c>
-      <c r="M32" s="15">
-        <v>4.3</v>
+      <c r="K32" s="14">
+        <v>3.9</v>
+      </c>
+      <c r="L32" s="14">
+        <v>3.1</v>
+      </c>
+      <c r="M32" s="14">
+        <v>3.1</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" s="14">
-        <v>6.2</v>
-      </c>
-      <c r="D33" s="14">
-        <v>5.5</v>
-      </c>
-      <c r="E33" s="14">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="F33" s="14">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="G33" s="14">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H33" s="18">
-        <v>4</v>
-      </c>
-      <c r="I33" s="14">
-        <v>3.3</v>
-      </c>
-      <c r="J33" s="14">
+        <v>80</v>
+      </c>
+      <c r="C33" s="15">
+        <v>5.4</v>
+      </c>
+      <c r="D33" s="15">
+        <v>5.2</v>
+      </c>
+      <c r="E33" s="15">
+        <v>4.7</v>
+      </c>
+      <c r="F33" s="15">
+        <v>4.7</v>
+      </c>
+      <c r="G33" s="15">
         <v>4.5</v>
       </c>
-      <c r="K33" s="14">
-        <v>3.9</v>
-      </c>
-      <c r="L33" s="14">
+      <c r="H33" s="15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I33" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="J33" s="15">
+        <v>3.7</v>
+      </c>
+      <c r="K33" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="L33" s="15">
         <v>3.1</v>
       </c>
-      <c r="M33" s="14">
-        <v>3.1</v>
+      <c r="M33" s="19">
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C34" s="15">
-        <v>5.4</v>
-      </c>
-      <c r="D34" s="15">
-        <v>5.2</v>
-      </c>
-      <c r="E34" s="15">
-        <v>4.7</v>
-      </c>
-      <c r="F34" s="15">
-        <v>4.7</v>
-      </c>
-      <c r="G34" s="15">
-        <v>4.5</v>
-      </c>
-      <c r="H34" s="15">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="I34" s="15">
+        <v>82</v>
+      </c>
+      <c r="C34" s="14">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D34" s="18">
+        <v>4</v>
+      </c>
+      <c r="E34" s="14">
         <v>3.5</v>
       </c>
-      <c r="J34" s="15">
-        <v>3.7</v>
-      </c>
-      <c r="K34" s="15">
-        <v>2.8</v>
-      </c>
-      <c r="L34" s="15">
+      <c r="F34" s="14">
+        <v>3.3</v>
+      </c>
+      <c r="G34" s="14">
+        <v>3.4</v>
+      </c>
+      <c r="H34" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="I34" s="14">
+        <v>2.6</v>
+      </c>
+      <c r="J34" s="14">
+        <v>3.8</v>
+      </c>
+      <c r="K34" s="14">
         <v>3.1</v>
       </c>
-      <c r="M34" s="19">
-        <v>3</v>
+      <c r="L34" s="14">
+        <v>2.6</v>
+      </c>
+      <c r="M34" s="14">
+        <v>2.6</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C35" s="14">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D35" s="18">
+        <v>84</v>
+      </c>
+      <c r="C35" s="19">
         <v>4</v>
       </c>
-      <c r="E35" s="14">
-        <v>3.5</v>
-      </c>
-      <c r="F35" s="14">
+      <c r="D35" s="15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E35" s="19">
+        <v>4</v>
+      </c>
+      <c r="F35" s="15">
+        <v>3.6</v>
+      </c>
+      <c r="G35" s="19">
+        <v>3</v>
+      </c>
+      <c r="H35" s="15">
+        <v>2.7</v>
+      </c>
+      <c r="I35" s="19">
+        <v>3</v>
+      </c>
+      <c r="J35" s="15">
         <v>3.3</v>
       </c>
-      <c r="G35" s="14">
-        <v>3.4</v>
-      </c>
-      <c r="H35" s="14">
+      <c r="K35" s="15">
+        <v>3.6</v>
+      </c>
+      <c r="L35" s="15">
+        <v>2.7</v>
+      </c>
+      <c r="M35" s="15">
         <v>2.5</v>
-      </c>
-      <c r="I35" s="14">
-        <v>2.6</v>
-      </c>
-      <c r="J35" s="14">
-        <v>3.8</v>
-      </c>
-      <c r="K35" s="14">
-        <v>3.1</v>
-      </c>
-      <c r="L35" s="14">
-        <v>2.6</v>
-      </c>
-      <c r="M35" s="14">
-        <v>2.6</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C36" s="19">
+        <v>86</v>
+      </c>
+      <c r="C36" s="14">
+        <v>6.4</v>
+      </c>
+      <c r="D36" s="14">
+        <v>6.4</v>
+      </c>
+      <c r="E36" s="14">
+        <v>5.9</v>
+      </c>
+      <c r="F36" s="14">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G36" s="14">
+        <v>4.3</v>
+      </c>
+      <c r="H36" s="14">
+        <v>4.3</v>
+      </c>
+      <c r="I36" s="14">
+        <v>3.8</v>
+      </c>
+      <c r="J36" s="14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="K36" s="14">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="L36" s="14">
+        <v>3.9</v>
+      </c>
+      <c r="M36" s="18">
         <v>4</v>
-      </c>
-      <c r="D36" s="15">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E36" s="19">
-        <v>4</v>
-      </c>
-      <c r="F36" s="15">
-        <v>3.6</v>
-      </c>
-      <c r="G36" s="19">
-        <v>3</v>
-      </c>
-      <c r="H36" s="15">
-        <v>2.7</v>
-      </c>
-      <c r="I36" s="19">
-        <v>3</v>
-      </c>
-      <c r="J36" s="15">
-        <v>3.3</v>
-      </c>
-      <c r="K36" s="15">
-        <v>3.6</v>
-      </c>
-      <c r="L36" s="15">
-        <v>2.7</v>
-      </c>
-      <c r="M36" s="15">
-        <v>2.5</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C37" s="14">
-        <v>6.4</v>
-      </c>
-      <c r="D37" s="14">
-        <v>6.4</v>
-      </c>
-      <c r="E37" s="14">
-        <v>5.9</v>
-      </c>
-      <c r="F37" s="14">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="G37" s="14">
-        <v>4.3</v>
-      </c>
-      <c r="H37" s="14">
-        <v>4.3</v>
-      </c>
-      <c r="I37" s="14">
-        <v>3.8</v>
-      </c>
-      <c r="J37" s="14">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="K37" s="14">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="L37" s="14">
+        <v>88</v>
+      </c>
+      <c r="C37" s="15">
+        <v>5.8</v>
+      </c>
+      <c r="D37" s="15">
+        <v>5.3</v>
+      </c>
+      <c r="E37" s="15">
+        <v>4.8</v>
+      </c>
+      <c r="F37" s="15">
         <v>3.9</v>
       </c>
-      <c r="M37" s="18">
-        <v>4</v>
+      <c r="G37" s="15">
+        <v>3.7</v>
+      </c>
+      <c r="H37" s="15">
+        <v>3.7</v>
+      </c>
+      <c r="I37" s="15">
+        <v>3.4</v>
+      </c>
+      <c r="J37" s="15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="K37" s="15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="L37" s="15">
+        <v>3.2</v>
+      </c>
+      <c r="M37" s="15">
+        <v>3.3</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C38" s="15">
-        <v>5.8</v>
-      </c>
-      <c r="D38" s="15">
-        <v>5.3</v>
-      </c>
-      <c r="E38" s="15">
-        <v>4.8</v>
-      </c>
-      <c r="F38" s="15">
+        <v>90</v>
+      </c>
+      <c r="C38" s="14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D38" s="14">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E38" s="14">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F38" s="14">
+        <v>4.3</v>
+      </c>
+      <c r="G38" s="14">
         <v>3.9</v>
       </c>
-      <c r="G38" s="15">
+      <c r="H38" s="14">
+        <v>3.6</v>
+      </c>
+      <c r="I38" s="14">
+        <v>3.4</v>
+      </c>
+      <c r="J38" s="14">
+        <v>3.6</v>
+      </c>
+      <c r="K38" s="14">
         <v>3.7</v>
       </c>
-      <c r="H38" s="15">
-        <v>3.7</v>
-      </c>
-      <c r="I38" s="15">
+      <c r="L38" s="14">
         <v>3.4</v>
       </c>
-      <c r="J38" s="15">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="K38" s="15">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="L38" s="15">
-        <v>3.2</v>
-      </c>
-      <c r="M38" s="15">
-        <v>3.3</v>
+      <c r="M38" s="18">
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" s="14">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="D39" s="14">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="E39" s="14">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="F39" s="14">
-        <v>4.3</v>
-      </c>
-      <c r="G39" s="14">
+        <v>92</v>
+      </c>
+      <c r="C39" s="19">
+        <v>5</v>
+      </c>
+      <c r="D39" s="19">
+        <v>5</v>
+      </c>
+      <c r="E39" s="15">
+        <v>4.7</v>
+      </c>
+      <c r="F39" s="15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G39" s="15">
         <v>3.9</v>
       </c>
-      <c r="H39" s="14">
-        <v>3.6</v>
-      </c>
-      <c r="I39" s="14">
-        <v>3.4</v>
-      </c>
-      <c r="J39" s="14">
-        <v>3.6</v>
-      </c>
-      <c r="K39" s="14">
+      <c r="H39" s="15">
+        <v>3.3</v>
+      </c>
+      <c r="I39" s="19">
+        <v>3</v>
+      </c>
+      <c r="J39" s="15">
         <v>3.7</v>
       </c>
-      <c r="L39" s="14">
-        <v>3.4</v>
-      </c>
-      <c r="M39" s="18">
-        <v>3</v>
+      <c r="K39" s="15">
+        <v>3.9</v>
+      </c>
+      <c r="L39" s="15">
+        <v>2.7</v>
+      </c>
+      <c r="M39" s="15">
+        <v>2.4</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C40" s="19">
+        <v>94</v>
+      </c>
+      <c r="C40" s="14">
+        <v>6.6</v>
+      </c>
+      <c r="D40" s="14">
+        <v>5.7</v>
+      </c>
+      <c r="E40" s="14">
+        <v>5.7</v>
+      </c>
+      <c r="F40" s="18">
         <v>5</v>
       </c>
-      <c r="D40" s="19">
-        <v>5</v>
-      </c>
-      <c r="E40" s="15">
+      <c r="G40" s="14">
         <v>4.7</v>
       </c>
-      <c r="F40" s="15">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="G40" s="15">
+      <c r="H40" s="18">
+        <v>4</v>
+      </c>
+      <c r="I40" s="14">
         <v>3.9</v>
       </c>
-      <c r="H40" s="15">
-        <v>3.3</v>
-      </c>
-      <c r="I40" s="19">
-        <v>3</v>
-      </c>
-      <c r="J40" s="15">
-        <v>3.7</v>
-      </c>
-      <c r="K40" s="15">
+      <c r="J40" s="14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="K40" s="14">
+        <v>4.2</v>
+      </c>
+      <c r="L40" s="14">
         <v>3.9</v>
       </c>
-      <c r="L40" s="15">
-        <v>2.7</v>
-      </c>
-      <c r="M40" s="15">
-        <v>2.4</v>
+      <c r="M40" s="14">
+        <v>3.6</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C41" s="14">
-        <v>6.6</v>
-      </c>
-      <c r="D41" s="14">
-        <v>5.7</v>
-      </c>
-      <c r="E41" s="14">
-        <v>5.7</v>
-      </c>
-      <c r="F41" s="18">
-        <v>5</v>
-      </c>
-      <c r="G41" s="14">
-        <v>4.7</v>
-      </c>
-      <c r="H41" s="18">
-        <v>4</v>
-      </c>
-      <c r="I41" s="14">
-        <v>3.9</v>
-      </c>
-      <c r="J41" s="14">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="K41" s="14">
-        <v>4.2</v>
-      </c>
-      <c r="L41" s="14">
-        <v>3.9</v>
-      </c>
-      <c r="M41" s="14">
-        <v>3.6</v>
+        <v>96</v>
+      </c>
+      <c r="C41" s="15">
+        <v>3.8</v>
+      </c>
+      <c r="D41" s="15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E41" s="15">
+        <v>3.4</v>
+      </c>
+      <c r="F41" s="15">
+        <v>3.4</v>
+      </c>
+      <c r="G41" s="15">
+        <v>3.1</v>
+      </c>
+      <c r="H41" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="I41" s="15">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="K41" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="L41" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="M41" s="15">
+        <v>2.5</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C42" s="15">
-        <v>3.8</v>
-      </c>
-      <c r="D42" s="15">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E42" s="15">
-        <v>3.4</v>
-      </c>
-      <c r="F42" s="15">
-        <v>3.4</v>
-      </c>
-      <c r="G42" s="15">
+        <v>98</v>
+      </c>
+      <c r="C42" s="14">
         <v>3.1</v>
       </c>
-      <c r="H42" s="15">
-        <v>2.8</v>
-      </c>
-      <c r="I42" s="15">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="J42" s="8" t="s">
+      <c r="D42" s="18">
+        <v>3</v>
+      </c>
+      <c r="E42" s="14">
+        <v>2.9</v>
+      </c>
+      <c r="F42" s="14">
+        <v>2.7</v>
+      </c>
+      <c r="G42" s="18">
+        <v>2</v>
+      </c>
+      <c r="H42" s="14">
+        <v>2.6</v>
+      </c>
+      <c r="I42" s="18">
+        <v>2</v>
+      </c>
+      <c r="J42" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="K42" s="15">
-        <v>2.8</v>
-      </c>
-      <c r="L42" s="15">
-        <v>2.8</v>
-      </c>
-      <c r="M42" s="15">
-        <v>2.5</v>
+      <c r="K42" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="L42" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="M42" s="7" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C43" s="14">
-        <v>3.1</v>
-      </c>
-      <c r="D43" s="18">
-        <v>3</v>
-      </c>
-      <c r="E43" s="14">
-        <v>2.9</v>
-      </c>
-      <c r="F43" s="14">
-        <v>2.7</v>
-      </c>
-      <c r="G43" s="18">
-        <v>2</v>
-      </c>
-      <c r="H43" s="14">
-        <v>2.6</v>
-      </c>
-      <c r="I43" s="18">
-        <v>2</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="K43" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="L43" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="M43" s="7" t="s">
-        <v>169</v>
+        <v>100</v>
+      </c>
+      <c r="C43" s="15">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D43" s="19">
+        <v>4</v>
+      </c>
+      <c r="E43" s="15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F43" s="15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G43" s="15">
+        <v>3.8</v>
+      </c>
+      <c r="H43" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="I43" s="15">
+        <v>3.3</v>
+      </c>
+      <c r="J43" s="19">
+        <v>4</v>
+      </c>
+      <c r="K43" s="15">
+        <v>4.2</v>
+      </c>
+      <c r="L43" s="15">
+        <v>3.6</v>
+      </c>
+      <c r="M43" s="15">
+        <v>3.6</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C44" s="15">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D44" s="19">
-        <v>4</v>
-      </c>
-      <c r="E44" s="15">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="F44" s="15">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="G44" s="15">
-        <v>3.8</v>
-      </c>
-      <c r="H44" s="15">
-        <v>3.5</v>
-      </c>
-      <c r="I44" s="15">
-        <v>3.3</v>
-      </c>
-      <c r="J44" s="19">
-        <v>4</v>
-      </c>
-      <c r="K44" s="15">
-        <v>4.2</v>
-      </c>
-      <c r="L44" s="15">
+        <v>102</v>
+      </c>
+      <c r="C44" s="18">
+        <v>6</v>
+      </c>
+      <c r="D44" s="14">
+        <v>5.8</v>
+      </c>
+      <c r="E44" s="14">
+        <v>5.6</v>
+      </c>
+      <c r="F44" s="14">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G44" s="14">
+        <v>4.5</v>
+      </c>
+      <c r="H44" s="14">
         <v>3.6</v>
       </c>
-      <c r="M44" s="15">
-        <v>3.6</v>
+      <c r="I44" s="14">
+        <v>3.7</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="K44" s="14">
+        <v>3.2</v>
+      </c>
+      <c r="L44" s="14">
+        <v>3.7</v>
+      </c>
+      <c r="M44" s="14">
+        <v>3.4</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C45" s="18">
-        <v>6</v>
-      </c>
-      <c r="D45" s="14">
-        <v>5.8</v>
-      </c>
-      <c r="E45" s="14">
-        <v>5.6</v>
-      </c>
-      <c r="F45" s="14">
+        <v>104</v>
+      </c>
+      <c r="C45" s="15">
+        <v>7.3</v>
+      </c>
+      <c r="D45" s="15">
+        <v>7.4</v>
+      </c>
+      <c r="E45" s="15">
+        <v>6.2</v>
+      </c>
+      <c r="F45" s="15">
         <v>4.9000000000000004</v>
       </c>
-      <c r="G45" s="14">
-        <v>4.5</v>
-      </c>
-      <c r="H45" s="14">
+      <c r="G45" s="15">
+        <v>4.3</v>
+      </c>
+      <c r="H45" s="15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I45" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="J45" s="15">
         <v>3.6</v>
       </c>
-      <c r="I45" s="14">
-        <v>3.7</v>
-      </c>
-      <c r="J45" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="K45" s="14">
-        <v>3.2</v>
-      </c>
-      <c r="L45" s="14">
-        <v>3.7</v>
-      </c>
-      <c r="M45" s="14">
+      <c r="K45" s="15">
         <v>3.4</v>
+      </c>
+      <c r="L45" s="15">
+        <v>3.4</v>
+      </c>
+      <c r="M45" s="15">
+        <v>2.4</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C46" s="15">
-        <v>7.3</v>
-      </c>
-      <c r="D46" s="15">
+        <v>106</v>
+      </c>
+      <c r="C46" s="14">
         <v>7.4</v>
       </c>
-      <c r="E46" s="15">
-        <v>6.2</v>
-      </c>
-      <c r="F46" s="15">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="G46" s="15">
-        <v>4.3</v>
-      </c>
-      <c r="H46" s="15">
+      <c r="D46" s="14">
+        <v>6.4</v>
+      </c>
+      <c r="E46" s="14">
+        <v>5.4</v>
+      </c>
+      <c r="F46" s="14">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G46" s="14">
         <v>4.0999999999999996</v>
       </c>
-      <c r="I46" s="15">
-        <v>3.5</v>
-      </c>
-      <c r="J46" s="15">
-        <v>3.6</v>
-      </c>
-      <c r="K46" s="15">
+      <c r="H46" s="14">
         <v>3.4</v>
       </c>
-      <c r="L46" s="15">
-        <v>3.4</v>
-      </c>
-      <c r="M46" s="15">
-        <v>2.4</v>
+      <c r="I46" s="14">
+        <v>3.7</v>
+      </c>
+      <c r="J46" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="K46" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L46" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="M46" s="14">
+        <v>3.3</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C47" s="14">
-        <v>7.4</v>
-      </c>
-      <c r="D47" s="14">
-        <v>6.4</v>
-      </c>
-      <c r="E47" s="14">
-        <v>5.4</v>
-      </c>
-      <c r="F47" s="14">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="G47" s="14">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="H47" s="14">
-        <v>3.4</v>
-      </c>
-      <c r="I47" s="14">
-        <v>3.7</v>
-      </c>
-      <c r="J47" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="K47" s="14">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="L47" s="14">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="M47" s="14">
-        <v>3.3</v>
+        <v>108</v>
+      </c>
+      <c r="C47" s="15">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D47" s="15">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E47" s="15">
+        <v>7.7</v>
+      </c>
+      <c r="F47" s="19">
+        <v>6</v>
+      </c>
+      <c r="G47" s="15">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H47" s="15">
+        <v>4.8</v>
+      </c>
+      <c r="I47" s="15">
+        <v>4.7</v>
+      </c>
+      <c r="J47" s="15">
+        <v>5.3</v>
+      </c>
+      <c r="K47" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="L47" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="M47" s="15">
+        <v>4.5</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C48" s="15">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="D48" s="15">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="E48" s="15">
-        <v>7.7</v>
-      </c>
-      <c r="F48" s="19">
-        <v>6</v>
-      </c>
-      <c r="G48" s="15">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="H48" s="15">
+        <v>110</v>
+      </c>
+      <c r="C48" s="14">
+        <v>9.1</v>
+      </c>
+      <c r="D48" s="14">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E48" s="18">
+        <v>8</v>
+      </c>
+      <c r="F48" s="14">
+        <v>7.4</v>
+      </c>
+      <c r="G48" s="14">
+        <v>6.9</v>
+      </c>
+      <c r="H48" s="14">
+        <v>5.3</v>
+      </c>
+      <c r="I48" s="14">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J48" s="14">
         <v>4.8</v>
       </c>
-      <c r="I48" s="15">
-        <v>4.7</v>
-      </c>
-      <c r="J48" s="15">
-        <v>5.3</v>
-      </c>
-      <c r="K48" s="15">
-        <v>4.5</v>
-      </c>
-      <c r="L48" s="15">
-        <v>3.5</v>
-      </c>
-      <c r="M48" s="15">
-        <v>4.5</v>
+      <c r="K48" s="14">
+        <v>4.2</v>
+      </c>
+      <c r="L48" s="14">
+        <v>3.9</v>
+      </c>
+      <c r="M48" s="14">
+        <v>3.8</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C49" s="14">
-        <v>9.1</v>
-      </c>
-      <c r="D49" s="14">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="E49" s="18">
-        <v>8</v>
-      </c>
-      <c r="F49" s="14">
-        <v>7.4</v>
-      </c>
-      <c r="G49" s="14">
-        <v>6.9</v>
-      </c>
-      <c r="H49" s="14">
-        <v>5.3</v>
-      </c>
-      <c r="I49" s="14">
+        <v>112</v>
+      </c>
+      <c r="C49" s="15">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D49" s="15">
         <v>4.5999999999999996</v>
       </c>
-      <c r="J49" s="14">
-        <v>4.8</v>
-      </c>
-      <c r="K49" s="14">
+      <c r="E49" s="15">
         <v>4.2</v>
       </c>
-      <c r="L49" s="14">
-        <v>3.9</v>
-      </c>
-      <c r="M49" s="14">
-        <v>3.8</v>
+      <c r="F49" s="19">
+        <v>4</v>
+      </c>
+      <c r="G49" s="15">
+        <v>3.6</v>
+      </c>
+      <c r="H49" s="15">
+        <v>3.1</v>
+      </c>
+      <c r="I49" s="15">
+        <v>2.9</v>
+      </c>
+      <c r="J49" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="K49" s="15">
+        <v>3.2</v>
+      </c>
+      <c r="L49" s="15">
+        <v>2.9</v>
+      </c>
+      <c r="M49" s="15">
+        <v>3.1</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C50" s="15">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="D50" s="15">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E50" s="15">
+        <v>114</v>
+      </c>
+      <c r="C50" s="18">
+        <v>6</v>
+      </c>
+      <c r="D50" s="18">
+        <v>6</v>
+      </c>
+      <c r="E50" s="14">
+        <v>5.8</v>
+      </c>
+      <c r="F50" s="14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="G50" s="14">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H50" s="14">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I50" s="14">
+        <v>3.7</v>
+      </c>
+      <c r="J50" s="14">
         <v>4.2</v>
       </c>
-      <c r="F50" s="19">
-        <v>4</v>
-      </c>
-      <c r="G50" s="15">
-        <v>3.6</v>
-      </c>
-      <c r="H50" s="15">
-        <v>3.1</v>
-      </c>
-      <c r="I50" s="15">
-        <v>2.9</v>
-      </c>
-      <c r="J50" s="15">
+      <c r="K50" s="14">
         <v>3.5</v>
       </c>
-      <c r="K50" s="15">
-        <v>3.2</v>
-      </c>
-      <c r="L50" s="15">
-        <v>2.9</v>
-      </c>
-      <c r="M50" s="15">
+      <c r="L50" s="18">
+        <v>3</v>
+      </c>
+      <c r="M50" s="14">
         <v>3.1</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C51" s="18">
-        <v>6</v>
-      </c>
-      <c r="D51" s="18">
-        <v>6</v>
-      </c>
-      <c r="E51" s="14">
-        <v>5.8</v>
-      </c>
-      <c r="F51" s="14">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="G51" s="14">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H51" s="14">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="I51" s="14">
-        <v>3.7</v>
-      </c>
-      <c r="J51" s="14">
-        <v>4.2</v>
-      </c>
-      <c r="K51" s="14">
-        <v>3.5</v>
-      </c>
-      <c r="L51" s="18">
-        <v>3</v>
-      </c>
-      <c r="M51" s="14">
-        <v>3.1</v>
+        <v>116</v>
+      </c>
+      <c r="C51" s="15">
+        <v>13.2</v>
+      </c>
+      <c r="D51" s="15">
+        <v>11.6</v>
+      </c>
+      <c r="E51" s="15">
+        <v>10.1</v>
+      </c>
+      <c r="F51" s="15">
+        <v>8.6</v>
+      </c>
+      <c r="G51" s="15">
+        <v>6.2</v>
+      </c>
+      <c r="H51" s="15">
+        <v>5.6</v>
+      </c>
+      <c r="I51" s="15">
+        <v>4.8</v>
+      </c>
+      <c r="J51" s="19">
+        <v>5</v>
+      </c>
+      <c r="K51" s="19">
+        <v>5</v>
+      </c>
+      <c r="L51" s="19">
+        <v>4</v>
+      </c>
+      <c r="M51" s="15">
+        <v>3.8</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C52" s="15">
-        <v>13.2</v>
-      </c>
-      <c r="D52" s="15">
-        <v>11.6</v>
-      </c>
-      <c r="E52" s="15">
-        <v>10.1</v>
-      </c>
-      <c r="F52" s="15">
+        <v>118</v>
+      </c>
+      <c r="C52" s="14">
+        <v>14.3</v>
+      </c>
+      <c r="D52" s="14">
+        <v>12.7</v>
+      </c>
+      <c r="E52" s="14">
+        <v>10.7</v>
+      </c>
+      <c r="F52" s="14">
         <v>8.6</v>
       </c>
-      <c r="G52" s="15">
+      <c r="G52" s="18">
+        <v>7</v>
+      </c>
+      <c r="H52" s="14">
         <v>6.2</v>
       </c>
-      <c r="H52" s="15">
-        <v>5.6</v>
-      </c>
-      <c r="I52" s="15">
-        <v>4.8</v>
-      </c>
-      <c r="J52" s="19">
-        <v>5</v>
-      </c>
-      <c r="K52" s="19">
-        <v>5</v>
-      </c>
-      <c r="L52" s="19">
-        <v>4</v>
-      </c>
-      <c r="M52" s="15">
-        <v>3.8</v>
+      <c r="I52" s="14">
+        <v>5.5</v>
+      </c>
+      <c r="J52" s="14">
+        <v>5.8</v>
+      </c>
+      <c r="K52" s="14">
+        <v>6.5</v>
+      </c>
+      <c r="L52" s="14">
+        <v>4.3</v>
+      </c>
+      <c r="M52" s="14">
+        <v>4.2</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C53" s="14">
-        <v>14.3</v>
-      </c>
-      <c r="D53" s="14">
-        <v>12.7</v>
-      </c>
-      <c r="E53" s="14">
-        <v>10.7</v>
-      </c>
-      <c r="F53" s="14">
-        <v>8.6</v>
-      </c>
-      <c r="G53" s="18">
-        <v>7</v>
-      </c>
-      <c r="H53" s="14">
-        <v>6.2</v>
-      </c>
-      <c r="I53" s="14">
-        <v>5.5</v>
-      </c>
-      <c r="J53" s="14">
+        <v>120</v>
+      </c>
+      <c r="C53" s="15">
+        <v>13.6</v>
+      </c>
+      <c r="D53" s="15">
+        <v>11.5</v>
+      </c>
+      <c r="E53" s="15">
+        <v>9.4</v>
+      </c>
+      <c r="F53" s="15">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G53" s="15">
+        <v>6.7</v>
+      </c>
+      <c r="H53" s="15">
+        <v>5.6</v>
+      </c>
+      <c r="I53" s="15">
+        <v>4.7</v>
+      </c>
+      <c r="J53" s="15">
         <v>5.8</v>
       </c>
-      <c r="K53" s="14">
+      <c r="K53" s="15">
         <v>6.5</v>
       </c>
-      <c r="L53" s="14">
-        <v>4.3</v>
-      </c>
-      <c r="M53" s="14">
-        <v>4.2</v>
+      <c r="L53" s="15">
+        <v>4.7</v>
+      </c>
+      <c r="M53" s="15">
+        <v>4.5</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C54" s="15">
-        <v>13.6</v>
-      </c>
-      <c r="D54" s="15">
-        <v>11.5</v>
-      </c>
-      <c r="E54" s="15">
-        <v>9.4</v>
-      </c>
-      <c r="F54" s="15">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="G54" s="15">
-        <v>6.7</v>
-      </c>
-      <c r="H54" s="15">
-        <v>5.6</v>
-      </c>
-      <c r="I54" s="15">
-        <v>4.7</v>
-      </c>
-      <c r="J54" s="15">
-        <v>5.8</v>
-      </c>
-      <c r="K54" s="15">
-        <v>6.5</v>
-      </c>
-      <c r="L54" s="15">
-        <v>4.7</v>
-      </c>
-      <c r="M54" s="15">
-        <v>4.5</v>
+        <v>122</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J54" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="K54" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="L54" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="M54" s="7" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C55" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="E55" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="F55" s="7" t="s">
+      <c r="F55" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="G55" s="7" t="s">
+      <c r="G55" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="H55" s="7" t="s">
+      <c r="H55" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="I55" s="7" t="s">
+      <c r="I55" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="J55" s="7" t="s">
+      <c r="J55" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="K55" s="7" t="s">
+      <c r="K55" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="L55" s="7" t="s">
+      <c r="L55" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="M55" s="7" t="s">
+      <c r="M55" s="8" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C56" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C56" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D56" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E56" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="F56" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="G56" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="H56" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="I56" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="J56" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="K56" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="L56" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="M56" s="8" t="s">
-        <v>169</v>
+      <c r="F56" s="14">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="G56" s="18">
+        <v>16</v>
+      </c>
+      <c r="H56" s="14">
+        <v>12.1</v>
+      </c>
+      <c r="I56" s="14">
+        <v>9.5</v>
+      </c>
+      <c r="J56" s="14">
+        <v>11.9</v>
+      </c>
+      <c r="K56" s="14">
+        <v>9.5</v>
+      </c>
+      <c r="L56" s="14">
+        <v>10.6</v>
+      </c>
+      <c r="M56" s="14">
+        <v>10.1</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="F57" s="14">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="G57" s="18">
-        <v>16</v>
-      </c>
-      <c r="H57" s="14">
-        <v>12.1</v>
-      </c>
-      <c r="I57" s="14">
-        <v>9.5</v>
-      </c>
-      <c r="J57" s="14">
-        <v>11.9</v>
-      </c>
-      <c r="K57" s="14">
-        <v>9.5</v>
-      </c>
-      <c r="L57" s="14">
-        <v>10.6</v>
-      </c>
-      <c r="M57" s="14">
-        <v>10.1</v>
+        <v>128</v>
+      </c>
+      <c r="C57" s="15">
+        <v>14.9</v>
+      </c>
+      <c r="D57" s="15">
+        <v>16.7</v>
+      </c>
+      <c r="E57" s="15">
+        <v>16.7</v>
+      </c>
+      <c r="F57" s="15">
+        <v>13.9</v>
+      </c>
+      <c r="G57" s="15">
+        <v>10.8</v>
+      </c>
+      <c r="H57" s="15">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I57" s="15">
+        <v>6.4</v>
+      </c>
+      <c r="J57" s="15">
+        <v>7.4</v>
+      </c>
+      <c r="K57" s="15">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L57" s="15">
+        <v>6.8</v>
+      </c>
+      <c r="M57" s="19">
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C58" s="15">
-        <v>14.9</v>
-      </c>
-      <c r="D58" s="15">
-        <v>16.7</v>
-      </c>
-      <c r="E58" s="15">
-        <v>16.7</v>
-      </c>
-      <c r="F58" s="15">
-        <v>13.9</v>
-      </c>
-      <c r="G58" s="15">
-        <v>10.8</v>
-      </c>
-      <c r="H58" s="15">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="I58" s="15">
-        <v>6.4</v>
-      </c>
-      <c r="J58" s="15">
-        <v>7.4</v>
-      </c>
-      <c r="K58" s="15">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="L58" s="15">
-        <v>6.8</v>
-      </c>
-      <c r="M58" s="19">
-        <v>6</v>
+        <v>130</v>
+      </c>
+      <c r="C58" s="14">
+        <v>18.3</v>
+      </c>
+      <c r="D58" s="14">
+        <v>17.5</v>
+      </c>
+      <c r="E58" s="14">
+        <v>15.9</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="I58" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J58" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="K58" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="L58" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="M58" s="7" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C59" s="14">
-        <v>18.3</v>
-      </c>
-      <c r="D59" s="14">
-        <v>17.5</v>
-      </c>
-      <c r="E59" s="14">
-        <v>15.9</v>
-      </c>
-      <c r="F59" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="G59" s="7" t="s">
+      <c r="D59" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="H59" s="7" t="s">
+      <c r="E59" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="I59" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="J59" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="K59" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="L59" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="M59" s="7" t="s">
-        <v>169</v>
+      <c r="F59" s="15">
+        <v>9.5</v>
+      </c>
+      <c r="G59" s="15">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="H59" s="15">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I59" s="15">
+        <v>5.4</v>
+      </c>
+      <c r="J59" s="15">
+        <v>4.7</v>
+      </c>
+      <c r="K59" s="15">
+        <v>5.3</v>
+      </c>
+      <c r="L59" s="15">
+        <v>5.3</v>
+      </c>
+      <c r="M59" s="15">
+        <v>3.8</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C60" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C60" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="D60" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="E60" s="8" t="s">
+      <c r="E60" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="F60" s="15">
-        <v>9.5</v>
-      </c>
-      <c r="G60" s="15">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="H60" s="15">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="I60" s="15">
-        <v>5.4</v>
-      </c>
-      <c r="J60" s="15">
-        <v>4.7</v>
-      </c>
-      <c r="K60" s="15">
-        <v>5.3</v>
-      </c>
-      <c r="L60" s="15">
-        <v>5.3</v>
-      </c>
-      <c r="M60" s="15">
-        <v>3.8</v>
+      <c r="F60" s="18">
+        <v>10</v>
+      </c>
+      <c r="G60" s="14">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="H60" s="14">
+        <v>5.8</v>
+      </c>
+      <c r="I60" s="14">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J60" s="18">
+        <v>5</v>
+      </c>
+      <c r="K60" s="14">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L60" s="18">
+        <v>4</v>
+      </c>
+      <c r="M60" s="14">
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="F61" s="18">
-        <v>10</v>
-      </c>
-      <c r="G61" s="14">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="H61" s="14">
-        <v>5.8</v>
-      </c>
-      <c r="I61" s="14">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="J61" s="18">
-        <v>5</v>
-      </c>
-      <c r="K61" s="14">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="L61" s="18">
-        <v>4</v>
-      </c>
-      <c r="M61" s="14">
-        <v>4.4000000000000004</v>
+        <v>136</v>
+      </c>
+      <c r="C61" s="15">
+        <v>7.4</v>
+      </c>
+      <c r="D61" s="15">
+        <v>7.5</v>
+      </c>
+      <c r="E61" s="15">
+        <v>7.5</v>
+      </c>
+      <c r="F61" s="15">
+        <v>7.6</v>
+      </c>
+      <c r="G61" s="15">
+        <v>7.9</v>
+      </c>
+      <c r="H61" s="15">
+        <v>7.5</v>
+      </c>
+      <c r="I61" s="15">
+        <v>7.5</v>
+      </c>
+      <c r="J61" s="15">
+        <v>7.7</v>
+      </c>
+      <c r="K61" s="15">
+        <v>7.6</v>
+      </c>
+      <c r="L61" s="15">
+        <v>6.6</v>
+      </c>
+      <c r="M61" s="15">
+        <v>6.7</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C62" s="15">
-        <v>7.4</v>
-      </c>
-      <c r="D62" s="15">
-        <v>7.5</v>
-      </c>
-      <c r="E62" s="15">
-        <v>7.5</v>
-      </c>
-      <c r="F62" s="15">
-        <v>7.6</v>
-      </c>
-      <c r="G62" s="15">
-        <v>7.9</v>
-      </c>
-      <c r="H62" s="15">
-        <v>7.5</v>
-      </c>
-      <c r="I62" s="15">
-        <v>7.5</v>
-      </c>
-      <c r="J62" s="15">
-        <v>7.7</v>
-      </c>
-      <c r="K62" s="15">
-        <v>7.6</v>
-      </c>
-      <c r="L62" s="15">
-        <v>6.6</v>
-      </c>
-      <c r="M62" s="15">
-        <v>6.7</v>
+        <v>138</v>
+      </c>
+      <c r="C62" s="14">
+        <v>4.2</v>
+      </c>
+      <c r="D62" s="14">
+        <v>4.5</v>
+      </c>
+      <c r="E62" s="14">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F62" s="14">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G62" s="14">
+        <v>4.2</v>
+      </c>
+      <c r="H62" s="14">
+        <v>4.3</v>
+      </c>
+      <c r="I62" s="14">
+        <v>3.8</v>
+      </c>
+      <c r="J62" s="14">
+        <v>4.3</v>
+      </c>
+      <c r="K62" s="14">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="L62" s="14">
+        <v>3.8</v>
+      </c>
+      <c r="M62" s="14">
+        <v>3.5</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C63" s="14">
-        <v>4.2</v>
-      </c>
-      <c r="D63" s="14">
-        <v>4.5</v>
-      </c>
-      <c r="E63" s="14">
+        <v>140</v>
+      </c>
+      <c r="C63" s="15">
         <v>4.4000000000000004</v>
       </c>
-      <c r="F63" s="14">
+      <c r="D63" s="15">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G63" s="14">
-        <v>4.2</v>
-      </c>
-      <c r="H63" s="14">
+      <c r="E63" s="15">
         <v>4.3</v>
       </c>
-      <c r="I63" s="14">
-        <v>3.8</v>
-      </c>
-      <c r="J63" s="14">
+      <c r="F63" s="19">
+        <v>5</v>
+      </c>
+      <c r="G63" s="15">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H63" s="15">
         <v>4.3</v>
       </c>
-      <c r="K63" s="14">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="L63" s="14">
-        <v>3.8</v>
-      </c>
-      <c r="M63" s="14">
+      <c r="I63" s="15">
         <v>3.5</v>
+      </c>
+      <c r="J63" s="15">
+        <v>4.8</v>
+      </c>
+      <c r="K63" s="15">
+        <v>4.8</v>
+      </c>
+      <c r="L63" s="15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="M63" s="15">
+        <v>3.9</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C64" s="15">
+        <v>142</v>
+      </c>
+      <c r="C64" s="14">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D64" s="15">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E64" s="15">
+      <c r="D64" s="14">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E64" s="14">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F64" s="14">
+        <v>3.9</v>
+      </c>
+      <c r="G64" s="14">
+        <v>4.5</v>
+      </c>
+      <c r="H64" s="14">
         <v>4.3</v>
       </c>
-      <c r="F64" s="19">
-        <v>5</v>
-      </c>
-      <c r="G64" s="15">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H64" s="15">
+      <c r="I64" s="18">
+        <v>4</v>
+      </c>
+      <c r="J64" s="14">
         <v>4.3</v>
       </c>
-      <c r="I64" s="15">
-        <v>3.5</v>
-      </c>
-      <c r="J64" s="15">
-        <v>4.8</v>
-      </c>
-      <c r="K64" s="15">
-        <v>4.8</v>
-      </c>
-      <c r="L64" s="15">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="M64" s="15">
-        <v>3.9</v>
+      <c r="K64" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="L64" s="14">
+        <v>3.7</v>
+      </c>
+      <c r="M64" s="14">
+        <v>3.4</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C65" s="14">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D65" s="14">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E65" s="14">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="F65" s="14">
+        <v>144</v>
+      </c>
+      <c r="C65" s="15">
         <v>3.9</v>
       </c>
-      <c r="G65" s="14">
-        <v>4.5</v>
-      </c>
-      <c r="H65" s="14">
-        <v>4.3</v>
-      </c>
-      <c r="I65" s="18">
+      <c r="D65" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="E65" s="19">
         <v>4</v>
       </c>
-      <c r="J65" s="14">
-        <v>4.3</v>
-      </c>
-      <c r="K65" s="14">
-        <v>4.7</v>
-      </c>
-      <c r="L65" s="14">
-        <v>3.7</v>
-      </c>
-      <c r="M65" s="14">
-        <v>3.4</v>
+      <c r="F65" s="19">
+        <v>4</v>
+      </c>
+      <c r="G65" s="15">
+        <v>3.8</v>
+      </c>
+      <c r="H65" s="15">
+        <v>3.6</v>
+      </c>
+      <c r="I65" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="J65" s="15">
+        <v>3.9</v>
+      </c>
+      <c r="K65" s="19">
+        <v>4</v>
+      </c>
+      <c r="L65" s="19">
+        <v>3</v>
+      </c>
+      <c r="M65" s="15">
+        <v>3.1</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C66" s="15">
-        <v>3.9</v>
-      </c>
-      <c r="D66" s="15">
-        <v>3.5</v>
-      </c>
-      <c r="E66" s="19">
-        <v>4</v>
-      </c>
-      <c r="F66" s="19">
-        <v>4</v>
-      </c>
-      <c r="G66" s="15">
-        <v>3.8</v>
-      </c>
-      <c r="H66" s="15">
-        <v>3.6</v>
-      </c>
-      <c r="I66" s="15">
-        <v>3.5</v>
-      </c>
-      <c r="J66" s="15">
-        <v>3.9</v>
-      </c>
-      <c r="K66" s="19">
-        <v>4</v>
-      </c>
-      <c r="L66" s="19">
-        <v>3</v>
-      </c>
-      <c r="M66" s="15">
-        <v>3.1</v>
+        <v>146</v>
+      </c>
+      <c r="C66" s="14">
+        <v>2.9</v>
+      </c>
+      <c r="D66" s="14">
+        <v>3.7</v>
+      </c>
+      <c r="E66" s="14">
+        <v>3.4</v>
+      </c>
+      <c r="F66" s="14">
+        <v>3.4</v>
+      </c>
+      <c r="G66" s="14">
+        <v>2.9</v>
+      </c>
+      <c r="H66" s="14">
+        <v>2.9</v>
+      </c>
+      <c r="I66" s="14">
+        <v>2.7</v>
+      </c>
+      <c r="J66" s="14">
+        <v>2.9</v>
+      </c>
+      <c r="K66" s="14">
+        <v>3.2</v>
+      </c>
+      <c r="L66" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="M66" s="14">
+        <v>2.7</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C67" s="14">
-        <v>2.9</v>
-      </c>
-      <c r="D67" s="14">
-        <v>3.7</v>
-      </c>
-      <c r="E67" s="14">
-        <v>3.4</v>
-      </c>
-      <c r="F67" s="14">
-        <v>3.4</v>
-      </c>
-      <c r="G67" s="14">
-        <v>2.9</v>
-      </c>
-      <c r="H67" s="14">
-        <v>2.9</v>
-      </c>
-      <c r="I67" s="14">
-        <v>2.7</v>
-      </c>
-      <c r="J67" s="14">
-        <v>2.9</v>
-      </c>
-      <c r="K67" s="14">
-        <v>3.2</v>
-      </c>
-      <c r="L67" s="14">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="M67" s="14">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B68" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="C68" s="15">
+      <c r="C67" s="15">
         <v>7.8</v>
       </c>
-      <c r="D68" s="15">
+      <c r="D67" s="15">
         <v>7.2</v>
       </c>
-      <c r="E68" s="15">
+      <c r="E67" s="15">
         <v>6.9</v>
       </c>
-      <c r="F68" s="15">
+      <c r="F67" s="15">
         <v>6.9</v>
       </c>
-      <c r="G68" s="15">
+      <c r="G67" s="15">
         <v>6.1</v>
       </c>
-      <c r="H68" s="15">
+      <c r="H67" s="15">
         <v>6.7</v>
       </c>
-      <c r="I68" s="15">
+      <c r="I67" s="15">
         <v>6.9</v>
       </c>
-      <c r="J68" s="15">
+      <c r="J67" s="15">
         <v>6.6</v>
       </c>
-      <c r="K68" s="19">
+      <c r="K67" s="19">
         <v>8</v>
       </c>
-      <c r="L68" s="15">
+      <c r="L67" s="15">
         <v>6.1</v>
       </c>
-      <c r="M68" s="15">
+      <c r="M67" s="15">
         <v>6.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>